<commit_message>
Adding invoice for board components, and updating expenditures
</commit_message>
<xml_diff>
--- a/Expenditures.xlsx
+++ b/Expenditures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjhal\Desktop\School\ECE 411\ECE411\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAB682D-FF46-45EB-9CEF-8B7AE0B997F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7B112-B0FA-4260-BECA-5797A4CC3A31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40953730-783B-46FA-952B-3DCB620ABCB6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>Items ordered</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Oct. 30</t>
+  </si>
+  <si>
+    <t>Oct.31</t>
+  </si>
+  <si>
+    <t>Board Components (See Component Invoice.xlsx)</t>
   </si>
 </sst>
 </file>
@@ -168,7 +174,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -191,6 +197,9 @@
     <xf numFmtId="8" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -512,7 +521,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -674,9 +683,15 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
+      <c r="M6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="13">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">

</xml_diff>

<commit_message>
Updated Expenditures and added Digi-Key order invoice
</commit_message>
<xml_diff>
--- a/Expenditures.xlsx
+++ b/Expenditures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjhal\Desktop\School\ECE 411\ECE411\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAB682D-FF46-45EB-9CEF-8B7AE0B997F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7B112-B0FA-4260-BECA-5797A4CC3A31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40953730-783B-46FA-952B-3DCB620ABCB6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>Items ordered</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Oct. 30</t>
+  </si>
+  <si>
+    <t>Oct.31</t>
+  </si>
+  <si>
+    <t>Board Components (See Component Invoice.xlsx)</t>
   </si>
 </sst>
 </file>
@@ -168,7 +174,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -191,6 +197,9 @@
     <xf numFmtId="8" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -512,7 +521,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -674,9 +683,15 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
+      <c r="M6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="13">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">

</xml_diff>

<commit_message>
Added breakouts to Bliss's expenditures
</commit_message>
<xml_diff>
--- a/Expenditures.xlsx
+++ b/Expenditures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Desktop\PSU\ECE 411\ECE411\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjhal\Desktop\ECE411\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFEB36B-73B4-4F00-A90A-82B41945B293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AB0163-C70E-410B-AB2E-8E930F818657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{40953730-783B-46FA-952B-3DCB620ABCB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40953730-783B-46FA-952B-3DCB620ABCB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>Items ordered</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Li-Ion Battery Pack</t>
+  </si>
+  <si>
+    <t>Atmega Breakout Board x2</t>
   </si>
 </sst>
 </file>
@@ -523,28 +526,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7BED87-D266-49DE-97E4-F6FE46834A37}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.26953125" customWidth="1"/>
-    <col min="9" max="9" width="17.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" customWidth="1"/>
-    <col min="12" max="12" width="5.81640625" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
     <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
@@ -566,7 +569,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:15" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,11 +607,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5"/>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5">
+        <v>29.88</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="E3" s="4" t="s">
         <v>17</v>
@@ -634,7 +639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -654,7 +659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -680,7 +685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -700,7 +705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -722,7 +727,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -736,7 +741,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -758,7 +763,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -772,7 +777,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -794,7 +799,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -808,7 +813,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -830,7 +835,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -844,7 +849,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -866,7 +871,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -880,7 +885,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -902,7 +907,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -916,7 +921,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -938,7 +943,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -952,7 +957,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>8</v>
       </c>

</xml_diff>